<commit_message>
Game over fade trigger
</commit_message>
<xml_diff>
--- a/Assets/Resources/Rainbow Road/rainbowroadxlsx.xlsx
+++ b/Assets/Resources/Rainbow Road/rainbowroadxlsx.xlsx
@@ -1,40 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Desktop\College\Software - Project 2 COMP313\Rhythm-Road\Assets\Audio\Songs\Rainbow Road\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Rhythm-Road\Rhythm-Road\Assets\Resources\Rainbow Road\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAA43B3-02D6-4273-8858-9F04493F36DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9460005B-5F46-495A-851B-7FD98B69B81F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rainbowroad" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="5">
   <si>
     <t>M</t>
   </si>
@@ -46,6 +33,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -886,10 +876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C254"/>
+  <dimension ref="A1:C255"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A241" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B258" sqref="B258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3685,6 +3675,17 @@
         <v>3</v>
       </c>
       <c r="C254">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>170000</v>
+      </c>
+      <c r="B255" t="s">
+        <v>4</v>
+      </c>
+      <c r="C255">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Game over screen functional accept letter colors
</commit_message>
<xml_diff>
--- a/Assets/Resources/Rainbow Road/rainbowroadxlsx.xlsx
+++ b/Assets/Resources/Rainbow Road/rainbowroadxlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Rhythm-Road\Rhythm-Road\Assets\Resources\Rainbow Road\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEAFABF-60E3-4AE5-9D4F-EE19B1E0DB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624F1A9B-5425-4730-BDF4-A0BE83DDA7C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="5">
   <si>
     <t>M</t>
   </si>
@@ -3696,10 +3696,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G292"/>
+  <dimension ref="A1:G293"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="M267" sqref="M267"/>
+    <sheetView tabSelected="1" topLeftCell="A274" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="N304" sqref="N304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3862,7 +3862,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" ref="A9:A28" si="2">A8+176</f>
+        <f t="shared" ref="A9:A27" si="2">A8+176</f>
         <v>4405</v>
       </c>
       <c r="B9" t="s">
@@ -8258,7 +8258,7 @@
         <v>1</v>
       </c>
       <c r="D242">
-        <f t="shared" ref="D242:D292" si="10">A242/1000</f>
+        <f t="shared" ref="D242:D293" si="10">A242/1000</f>
         <v>134.64099999999999</v>
       </c>
       <c r="E242">
@@ -9214,6 +9214,21 @@
       <c r="E292">
         <f t="shared" si="11"/>
         <v>1.5879999999999939</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>170000</v>
+      </c>
+      <c r="B293" t="s">
+        <v>4</v>
+      </c>
+      <c r="C293">
+        <v>1</v>
+      </c>
+      <c r="D293">
+        <f t="shared" si="10"/>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>